<commit_message>
Add additional custom hacks
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -411,209 +411,36 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Another Super Mario 3D</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>Skawo</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>Super Mario 64 DS</v>
+        <v/>
       </c>
       <c r="D2" t="str">
-        <v>NDS</v>
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>June 26, 2014</v>
+        <v/>
       </c>
       <c r="H2" t="b">
         <v>1</v>
       </c>
       <c r="I2" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Another_Super_Mario_3D</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Super Mario Star World</v>
-      </c>
-      <c r="B3" t="str">
-        <v>SKELUX</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D3" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Super_Mario_Star_World</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Super Mario 64 DS 2: The Next Journey</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Splatterboy</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D4" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G4" t="str">
-        <v>August 26, 2018</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Super_Mario_64_DS_2:_The_Next_Journey</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Excerpt from Super Mario 256</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Josh65536</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D5" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G5" t="str">
-        <v>December 15, 2018</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Excerpt_from_Super_Mario_256</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Super Mario 64 Shining Stars DS</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Gota7</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D6" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G6" t="str">
-        <v>June 2, 2022</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Super_Mario_64_Shining_Stars_DS</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Super Mario Journey Lane DS</v>
-      </c>
-      <c r="B7" t="str">
-        <v>ShaneMGD</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D7" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Super_Mario_Journey_Lane_DS</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Mario's Star Quest</v>
-      </c>
-      <c r="B8" t="str">
-        <v>oreo</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D8" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G8" t="str">
-        <v>August 11, 2020</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Mario%27s_Star_Quest</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Mario's Holiday</v>
-      </c>
-      <c r="B9" t="str">
-        <v>SKELUX</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D9" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G9" t="str">
-        <v>January 30, 2018</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Mario%27s_Holiday</v>
-      </c>
-    </row>
-    <row r="10" xml:space="preserve">
-      <c r="A10" t="str">
-        <v>Super Mario 64 DS with FLUDD</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Modified</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Super Mario 64 DS</v>
-      </c>
-      <c r="D10" t="str">
-        <v>NDS</v>
-      </c>
-      <c r="G10" t="str" xml:space="preserve">
-        <v xml:space="preserve">v1: December 11, 2018
-v2: May 19, 2020</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="str">
-        <v>https://mario64hacks.fandom.com/wiki/Super_Mario_64_DS_with_FLUDD</v>
+        <v>http://www.arcadecollecting.com/hacks/bagman/</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>